<commit_message>
updated code for utg-8
</commit_message>
<xml_diff>
--- a/email-list.xlsx
+++ b/email-list.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ultra\OneDrive\Personal Projects\Personal\Send Emails from CSV\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\vanags\sendmail-from-excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="36" documentId="8_{0FAA3405-A8DF-471E-9E62-B703C96B923B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{3767D45E-27FC-4DD0-9813-EF010EDFA5D6}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{64DA8388-E216-42B9-A611-4330A70C578A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11685" windowHeight="4635"/>
   </bookViews>
   <sheets>
     <sheet name="Email-List" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
   <si>
     <t>Email</t>
   </si>
@@ -42,34 +41,28 @@
     <t>Recipient Last Name</t>
   </si>
   <si>
-    <t>johndoe123@gmail.com</t>
-  </si>
-  <si>
-    <t>John</t>
-  </si>
-  <si>
     <t>Doe</t>
   </si>
   <si>
-    <t>Jane</t>
-  </si>
-  <si>
-    <t>janedoe321@yahoo.com</t>
-  </si>
-  <si>
-    <t>thisisanemail@gmail.com</t>
-  </si>
-  <si>
-    <t>Bob</t>
-  </si>
-  <si>
     <t>Green</t>
+  </si>
+  <si>
+    <t>raimunds.vanags@gmail.com</t>
+  </si>
+  <si>
+    <t>daily.com</t>
+  </si>
+  <si>
+    <t>news.com</t>
+  </si>
+  <si>
+    <t>kkas.co.uk</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -425,11 +418,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66395B03-A72A-434C-BDA6-F9DE4C5D1560}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -452,42 +445,42 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
         <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{12E51237-1BDF-414B-B741-A32D2C4C65AD}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{45B9962A-1FDD-49BC-877A-A7D42F8C41BA}"/>
-    <hyperlink ref="A4" r:id="rId3" xr:uid="{5150F6AA-2F9A-47AB-9CDA-FC777F04D4CC}"/>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="A4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>